<commit_message>
Updated Backlog Produit & Sprint Backlog
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A9A3EB-E3DA-4FF5-A493-3A64FF498AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7429AF-A74D-4BBD-80EB-7A139EA1B829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
-    <sheet name="PROJECT DETAILS" sheetId="4" state="hidden" r:id="rId2"/>
-    <sheet name="RESOURCES" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="6" r:id="rId2"/>
+    <sheet name="PROJECT DETAILS" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="RESOURCES" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
   <si>
     <t>Theme</t>
   </si>
@@ -101,12 +102,6 @@
   </si>
   <si>
     <t>Business Value</t>
-  </si>
-  <si>
-    <t>VC-US-1</t>
-  </si>
-  <si>
-    <t>Définir les critères pour la catégorie client</t>
   </si>
   <si>
     <t>Établir les critères pour déterminer si un client est classé en tant que VIP ou Standard en fonction de la valeur commerciale. Par exemple, définir les seuils de dépenses annuelles pour chaque catégorie.</t>
@@ -119,22 +114,10 @@
     <t>À faire</t>
   </si>
   <si>
-    <t>VC-US-2</t>
-  </si>
-  <si>
-    <t>Définir les critères d'offre pour évaluer la valeur commerciale</t>
-  </si>
-  <si>
     <t>Déterminer les critères d'offre, tels que le type de service (XDSL, HD), pour évaluer la valeur commerciale d'un client.</t>
   </si>
   <si>
     <t>Critères d'offre HD, XDSL</t>
-  </si>
-  <si>
-    <t>VC-US-3</t>
-  </si>
-  <si>
-    <t>Établir les critères de débit pour évaluer la valeur commerciale</t>
   </si>
   <si>
     <t>Définir les critères de débit (100, 50, 30, 20, 12, 10, 8, 4) pour évaluer la valeur commerciale d'un client en fonction de sa connexion.</t>
@@ -149,24 +132,12 @@
  4</t>
   </si>
   <si>
-    <t>VC-US-4</t>
-  </si>
-  <si>
-    <t>Identifier les critères d'engagement contractuel pour la valeur commerciale</t>
-  </si>
-  <si>
     <t>Déterminer les critères d'engagement contractuel (période d'engagement, non engagé) pour évaluer la valeur commerciale d'un client.</t>
   </si>
   <si>
     <t>Critères d'engagement contractuel 
  période d engagement 
  non engagé</t>
-  </si>
-  <si>
-    <t>EC-US-1</t>
-  </si>
-  <si>
-    <t>Définir les critères d'ancienneté pour l'engagement client</t>
   </si>
   <si>
     <t>Spécifier les critères d'ancienneté (2 ans et plus, 1 an à 2 ans, moins d'un an) pour évaluer l'engagement d'un client envers l'entreprise.</t>
@@ -178,12 +149,6 @@
  &lt;1 ans</t>
   </si>
   <si>
-    <t>EC-US-2</t>
-  </si>
-  <si>
-    <t>Établir les critères d'engagement client basés sur le montant de l'encours</t>
-  </si>
-  <si>
     <t>Définir les critères d'engagement client en fonction du montant de l'encours. Par exemple, déterminer si un client a moins de 2 factures impayées, aucune facture impayée ou une seule facture impayée.</t>
   </si>
   <si>
@@ -193,12 +158,6 @@
  une facture</t>
   </si>
   <si>
-    <t>EC-US-3</t>
-  </si>
-  <si>
-    <t>Identifier les critères d'engagement client liés aux suspensions de service</t>
-  </si>
-  <si>
     <t>Définir les critères d'engagement client en fonction du nombre de suspensions de service par an. Par exemple, déterminer si un client a été suspendu moins de 2 fois par an ou plus de 2 fois par an</t>
   </si>
   <si>
@@ -211,12 +170,6 @@
     <t>Réclamations clients</t>
   </si>
   <si>
-    <t>ET-US-1</t>
-  </si>
-  <si>
-    <t>Identifier les critères d'engagement TOPNET basés sur le délai de traitement des réclamations</t>
-  </si>
-  <si>
     <t>Définir les critères d'engagement TOPNET en fonction du délai de traitement des réclamations. Par exemple, déterminer si un client a un délai de traitement de réclamation supérieur ou inférieur au délai théorique de traitement.</t>
   </si>
   <si>
@@ -229,20 +182,11 @@
     <t>Délai de traitement des réclamations</t>
   </si>
   <si>
-    <t>ET-US-2</t>
-  </si>
-  <si>
     <t>Critères d'engagement TOPNET 
  &gt; Délai théorique de traitement de récl 
  &lt; Délai théorique de traitement de récl</t>
   </si>
   <si>
-    <t>CC-US-1</t>
-  </si>
-  <si>
-    <t>Définir les critères de délai moyen de paiement pour évaluer le comportement du client</t>
-  </si>
-  <si>
     <t>Spécifier les critères de délai moyen de paiement (inférieur à 30 jours, supérieur à 30 jours) pour évaluer le comportement de paiement d'un client.</t>
   </si>
   <si>
@@ -251,12 +195,6 @@
  Délai moyen de paiement&gt;30 j</t>
   </si>
   <si>
-    <t>CC-US-2</t>
-  </si>
-  <si>
-    <t>Identifier les critères d'incident de paiement pour évaluer le comportement du client</t>
-  </si>
-  <si>
     <t>Déterminer les critères d'incident de paiement (rejet ou non) pour évaluer le comportement de paiement d'un client.</t>
   </si>
   <si>
@@ -264,12 +202,6 @@
  incident de paiement( Rejet ) Oui Ou Non</t>
   </si>
   <si>
-    <t>CC-US-3</t>
-  </si>
-  <si>
-    <t>Définir les critères de contentieux pour évaluer le comportement du client</t>
-  </si>
-  <si>
     <t>Établir les critères de contentieux (oui ou non) pour évaluer le comportement du client en termes de litiges ou de poursuites.</t>
   </si>
   <si>
@@ -307,9 +239,6 @@
     <t>Project Management Templates</t>
   </si>
   <si>
-    <t>Regroupement d'Objectifs</t>
-  </si>
-  <si>
     <t>3 Jours</t>
   </si>
   <si>
@@ -378,13 +307,103 @@
   </si>
   <si>
     <t xml:space="preserve">ID  Du l'Item  </t>
+  </si>
+  <si>
+    <t>VC-I-1</t>
+  </si>
+  <si>
+    <t>VC-I-2</t>
+  </si>
+  <si>
+    <t>VC-I-3</t>
+  </si>
+  <si>
+    <t>VC-I-4</t>
+  </si>
+  <si>
+    <t>EC-I-1</t>
+  </si>
+  <si>
+    <t>EC-I-2</t>
+  </si>
+  <si>
+    <t>EC-I-3</t>
+  </si>
+  <si>
+    <t>ET-I-1</t>
+  </si>
+  <si>
+    <t>ET-I-2</t>
+  </si>
+  <si>
+    <t>CC-I-1</t>
+  </si>
+  <si>
+    <t>CC-I-2</t>
+  </si>
+  <si>
+    <t>CC-I-3</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peuxDéfinir les critères pour la catégorie client</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peux  Définir les critères d'offre pour évaluer la valeur commerciale</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet  je peux Établir les critères de débit pour évaluer la valeur commerciale</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peux  Identifier les critères d'engagement contractuel pour la valeur commerciale</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet  je peux Définir les critères d'ancienneté pour l'engagement client</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peux Établir les critères d'engagement client basés sur le montant de l'encours</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet  je peux Identifier les critères d'engagement client liés aux suspensions de service</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet  je peux Identifier les critères d'engagement TOPNET basés sur le délai de traitement des réclamations</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peux Identifier les critères d'engagement TOPNET basés sur le délai de traitement des réclamations</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peux Définir les critères de délai moyen de paiement pour évaluer le comportement du client</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peux Identifier les critères d'incident de paiement pour évaluer le comportement du client</t>
+  </si>
+  <si>
+    <t>En tant qu' Agent Du Topnet je peux Définir les critères de contentieux pour évaluer le comportement du client</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Somme</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Résultat cumulé</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimation de Priorité </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +506,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="26">
@@ -781,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -858,13 +884,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -929,6 +949,26 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,10 +1188,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AC13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="58" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1159,31 +1199,31 @@
     <col min="1" max="1" width="64.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" customWidth="1"/>
-    <col min="4" max="4" width="206" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="240" customWidth="1"/>
+    <col min="5" max="5" width="149.85546875" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
-    <col min="7" max="7" width="52.85546875" customWidth="1"/>
+    <col min="7" max="7" width="126.42578125" customWidth="1"/>
     <col min="8" max="8" width="43.7109375" customWidth="1"/>
     <col min="9" max="9" width="44.28515625" customWidth="1"/>
     <col min="10" max="10" width="47.85546875" customWidth="1"/>
     <col min="11" max="11" width="46.7109375" customWidth="1"/>
-    <col min="12" max="27" width="14.42578125" hidden="1"/>
+    <col min="12" max="27" width="14.42578125" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="145.140625" customWidth="1"/>
     <col min="29" max="29" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>1</v>
@@ -1191,20 +1231,14 @@
       <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>18</v>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>3</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1222,44 +1256,34 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-      <c r="AB1" s="1" t="s">
-        <v>103</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:27" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="74" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="F2" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="47">
-        <f t="shared" ref="H2:H13" si="0">J:J/I:I</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="I2" s="49">
+      <c r="G2" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="45">
+        <v>50</v>
+      </c>
+      <c r="I2" s="47">
         <v>60</v>
-      </c>
-      <c r="J2" s="19">
-        <v>80</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>89</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1277,42 +1301,32 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
-      <c r="AB2" s="64" t="s">
-        <v>94</v>
-      </c>
     </row>
-    <row r="3" spans="1:28" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="77"/>
+    <row r="3" spans="1:27" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="75"/>
       <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="45">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="I3" s="50">
+      <c r="G3" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="43">
         <v>40</v>
       </c>
-      <c r="J3" s="61">
-        <v>60</v>
-      </c>
-      <c r="K3" s="63" t="s">
-        <v>90</v>
+      <c r="I3" s="48">
+        <v>40</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1330,42 +1344,32 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="65" t="s">
-        <v>91</v>
-      </c>
     </row>
-    <row r="4" spans="1:28" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="77"/>
+    <row r="4" spans="1:27" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="75"/>
       <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="48">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="I4" s="51">
+        <v>83</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="46">
+        <v>10</v>
+      </c>
+      <c r="I4" s="49">
         <v>50</v>
-      </c>
-      <c r="J4" s="62">
-        <v>40</v>
-      </c>
-      <c r="K4" s="62" t="s">
-        <v>85</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -1383,42 +1387,32 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
-      <c r="AB4" s="66" t="s">
-        <v>92</v>
-      </c>
     </row>
-    <row r="5" spans="1:28" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="78"/>
+    <row r="5" spans="1:27" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="76"/>
       <c r="B5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="46">
-        <f t="shared" si="0"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="I5" s="52">
+        <v>84</v>
+      </c>
+      <c r="D5" s="82" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="44">
+        <v>60</v>
+      </c>
+      <c r="I5" s="50">
         <v>70</v>
-      </c>
-      <c r="J5" s="22">
-        <v>60</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1436,44 +1430,34 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
-      <c r="AB5" s="67" t="s">
-        <v>93</v>
-      </c>
     </row>
-    <row r="6" spans="1:28" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="79" t="s">
+    <row r="6" spans="1:27" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="77" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I6" s="53">
-        <v>80</v>
-      </c>
-      <c r="J6" s="23">
-        <v>80</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="D6" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="35">
+        <v>70</v>
+      </c>
+      <c r="I6" s="51">
+        <v>60</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -1491,79 +1475,59 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
-      <c r="AB6" s="75" t="s">
-        <v>96</v>
-      </c>
     </row>
-    <row r="7" spans="1:28" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="77"/>
+    <row r="7" spans="1:27" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="75"/>
       <c r="B7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="38">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="I7" s="54">
-        <v>90</v>
-      </c>
-      <c r="J7" s="31">
-        <v>60</v>
-      </c>
-      <c r="K7" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB7" s="68" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="D7" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="36">
+        <v>30</v>
+      </c>
+      <c r="I7" s="52">
+        <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="78"/>
+    <row r="8" spans="1:27" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="76"/>
       <c r="B8" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="39">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="I8" s="55">
+        <v>87</v>
+      </c>
+      <c r="D8" s="85" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="37">
+        <v>80</v>
+      </c>
+      <c r="I8" s="53">
         <v>60</v>
-      </c>
-      <c r="J8" s="32">
-        <v>40</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>84</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -1581,44 +1545,34 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
-      <c r="AB8" s="69" t="s">
-        <v>97</v>
-      </c>
     </row>
-    <row r="9" spans="1:28" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80" t="s">
+    <row r="9" spans="1:27" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="78" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="40">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="I9" s="56">
+        <v>88</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="38">
+        <v>40</v>
+      </c>
+      <c r="I9" s="54">
         <v>50</v>
-      </c>
-      <c r="J9" s="26">
-        <v>90</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>85</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1636,42 +1590,32 @@
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
-      <c r="AB9" s="70" t="s">
-        <v>98</v>
-      </c>
     </row>
-    <row r="10" spans="1:28" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="78"/>
+    <row r="10" spans="1:27" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="76"/>
       <c r="B10" s="27" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="41">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="I10" s="57">
+        <v>89</v>
+      </c>
+      <c r="D10" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="39">
+        <v>10</v>
+      </c>
+      <c r="I10" s="55">
         <v>40</v>
-      </c>
-      <c r="J10" s="27">
-        <v>60</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>85</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
@@ -1689,44 +1633,34 @@
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
       <c r="AA10" s="9"/>
-      <c r="AB10" s="71" t="s">
-        <v>99</v>
-      </c>
     </row>
-    <row r="11" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+    <row r="11" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="79" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="42">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I11" s="58">
+        <v>90</v>
+      </c>
+      <c r="D11" s="88" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="40">
+        <v>20</v>
+      </c>
+      <c r="I11" s="56">
         <v>30</v>
-      </c>
-      <c r="J11" s="28">
-        <v>60</v>
-      </c>
-      <c r="K11" s="28" t="s">
-        <v>86</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -1744,42 +1678,32 @@
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
-      <c r="AB11" s="72" t="s">
-        <v>100</v>
-      </c>
     </row>
-    <row r="12" spans="1:28" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="77"/>
+    <row r="12" spans="1:27" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="75"/>
       <c r="B12" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="43">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="59">
-        <v>40</v>
-      </c>
-      <c r="J12" s="29">
-        <v>40</v>
-      </c>
-      <c r="K12" s="29" t="s">
-        <v>86</v>
+        <v>91</v>
+      </c>
+      <c r="D12" s="89" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="41">
+        <v>10</v>
+      </c>
+      <c r="I12" s="57">
+        <v>30</v>
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
@@ -1797,42 +1721,32 @@
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
       <c r="AA12" s="11"/>
-      <c r="AB12" s="73" t="s">
-        <v>101</v>
-      </c>
     </row>
-    <row r="13" spans="1:28" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="78"/>
+    <row r="13" spans="1:27" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="76"/>
       <c r="B13" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="44">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="I13" s="60">
+        <v>92</v>
+      </c>
+      <c r="D13" s="90" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="42">
+        <v>10</v>
+      </c>
+      <c r="I13" s="58">
         <v>30</v>
-      </c>
-      <c r="J13" s="30">
-        <v>20</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>87</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -1850,9 +1764,6 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
-      <c r="AB13" s="74" t="s">
-        <v>102</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1861,19 +1772,280 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I13" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I13" xr:uid="{86B5F61D-41F8-4621-A960-58147D9E9B9D}">
       <formula1>"10,20,30,40,50,60,70,80,90,100"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G13" xr:uid="{00000000-0002-0000-0200-000001000000}">
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E318A1A-E033-4B72-B240-50A0F2C09518}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="B1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="62.85546875" customWidth="1"/>
+    <col min="5" max="5" width="82.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="45">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="C2" s="47">
+        <v>60</v>
+      </c>
+      <c r="D2" s="19">
+        <v>80</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="43">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="48">
+        <v>40</v>
+      </c>
+      <c r="D3" s="59">
+        <v>60</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="46">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="49">
+        <v>50</v>
+      </c>
+      <c r="D4" s="60">
+        <v>40</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="44">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="C5" s="50">
+        <v>70</v>
+      </c>
+      <c r="D5" s="22">
+        <v>60</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="35">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="51">
+        <v>80</v>
+      </c>
+      <c r="D6" s="23">
+        <v>80</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="36">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C7" s="52">
+        <v>90</v>
+      </c>
+      <c r="D7" s="31">
+        <v>60</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="37">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C8" s="53">
+        <v>60</v>
+      </c>
+      <c r="D8" s="32">
+        <v>40</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="38">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>1.8</v>
+      </c>
+      <c r="C9" s="54">
+        <v>50</v>
+      </c>
+      <c r="D9" s="26">
+        <v>90</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="39">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="55">
+        <v>40</v>
+      </c>
+      <c r="D10" s="27">
+        <v>60</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="40">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>2</v>
+      </c>
+      <c r="C11" s="56">
+        <v>30</v>
+      </c>
+      <c r="D11" s="28">
+        <v>60</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="41">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="57">
+        <v>40</v>
+      </c>
+      <c r="D12" s="29">
+        <v>40</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="42">
+        <f>D$1:D$13/C$1:C$13</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C13" s="58">
+        <v>30</v>
+      </c>
+      <c r="D13" s="30">
+        <v>20</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A13" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"À faire,En Cours ,Réalisé"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C13" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>"10,20,30,40,50,60,70,80,90,100"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF2F5496"/>
@@ -1894,7 +2066,7 @@
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="13"/>
@@ -1924,7 +2096,7 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="13"/>
@@ -1954,7 +2126,7 @@
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="13"/>
@@ -1984,7 +2156,7 @@
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="13"/>
@@ -3024,7 +3196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -3042,33 +3214,33 @@
   <sheetData>
     <row r="2" spans="1:26" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="17" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>

</xml_diff>

<commit_message>
TBP / TSB Scoring   , Journal
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AB76EF-C91B-4C57-8759-721957D580A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E8BBA-F88D-4FB2-BD90-17086A234092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -751,7 +751,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,12 +768,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF980000"/>
         <bgColor rgb="FF980000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0B5394"/>
-        <bgColor rgb="FF0B5394"/>
       </patternFill>
     </fill>
     <fill>
@@ -814,20 +808,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA64D79"/>
-        <bgColor rgb="FFA64D79"/>
       </patternFill>
     </fill>
     <fill>
@@ -840,12 +822,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD5A6BD"/>
         <bgColor rgb="FFD5A6BD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1C232"/>
-        <bgColor rgb="FFF1C232"/>
       </patternFill>
     </fill>
     <fill>
@@ -868,38 +844,110 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FF0B5394"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF6D9EEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF3C78D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FF980000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor rgb="FFC9DAF8"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor rgb="FFA4C2F4"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor rgb="FF3C78D8"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FFA64D79"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor rgb="FF3C78D8"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FFEAD1DC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor rgb="FF3C78D8"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD5A6BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFF1C232"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
   </fills>
@@ -1063,20 +1111,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1095,177 +1143,222 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,8 +1584,8 @@
   </sheetPr>
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="58" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="58" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1607,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -1559,31 +1652,31 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="61" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="45">
+      <c r="H2" s="61">
         <v>50</v>
       </c>
-      <c r="I2" s="47">
+      <c r="I2" s="63">
         <v>60</v>
       </c>
       <c r="L2" s="2"/>
@@ -1604,29 +1697,29 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="105"/>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="64"/>
+      <c r="B3" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="67">
         <v>40</v>
       </c>
-      <c r="I3" s="48">
+      <c r="I3" s="69">
         <v>40</v>
       </c>
       <c r="L3" s="3"/>
@@ -1647,29 +1740,29 @@
       <c r="AA3" s="3"/>
     </row>
     <row r="4" spans="1:27" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="87"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="70"/>
+      <c r="B4" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="74">
         <v>10</v>
       </c>
-      <c r="I4" s="49">
+      <c r="I4" s="76">
         <v>50</v>
       </c>
       <c r="L4" s="4"/>
@@ -1690,29 +1783,29 @@
       <c r="AA4" s="4"/>
     </row>
     <row r="5" spans="1:27" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="88"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="77"/>
+      <c r="B5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="44">
+      <c r="H5" s="80">
         <v>60</v>
       </c>
-      <c r="I5" s="50">
+      <c r="I5" s="82">
         <v>70</v>
       </c>
       <c r="L5" s="5"/>
@@ -1733,31 +1826,31 @@
       <c r="AA5" s="5"/>
     </row>
     <row r="6" spans="1:27" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="86">
         <v>70</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="88">
         <v>60</v>
       </c>
       <c r="L6" s="6"/>
@@ -1778,56 +1871,56 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="7" spans="1:27" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="87"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="66" t="s">
+      <c r="G7" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="92">
         <v>30</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="93">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="88"/>
-      <c r="B8" s="25" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="67" t="s">
+      <c r="G8" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="97">
         <v>80</v>
       </c>
-      <c r="I8" s="53">
+      <c r="I8" s="99">
         <v>60</v>
       </c>
       <c r="L8" s="7"/>
@@ -1848,31 +1941,31 @@
       <c r="AA8" s="7"/>
     </row>
     <row r="9" spans="1:27" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="101" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="80" t="s">
+      <c r="D9" s="102" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="103">
         <v>40</v>
       </c>
-      <c r="I9" s="54">
+      <c r="I9" s="105">
         <v>50</v>
       </c>
       <c r="L9" s="8"/>
@@ -1893,29 +1986,29 @@
       <c r="AA9" s="8"/>
     </row>
     <row r="10" spans="1:27" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="88"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="77"/>
+      <c r="B10" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="106" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="69" t="s">
+      <c r="G10" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="108">
         <v>10</v>
       </c>
-      <c r="I10" s="55">
+      <c r="I10" s="110">
         <v>40</v>
       </c>
       <c r="L10" s="9"/>
@@ -1936,31 +2029,31 @@
       <c r="AA10" s="9"/>
     </row>
     <row r="11" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="112" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="D11" s="113" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="70" t="s">
+      <c r="G11" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="114">
         <v>20</v>
       </c>
-      <c r="I11" s="56">
+      <c r="I11" s="116">
         <v>30</v>
       </c>
       <c r="L11" s="10"/>
@@ -1981,29 +2074,29 @@
       <c r="AA11" s="10"/>
     </row>
     <row r="12" spans="1:27" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="87"/>
-      <c r="B12" s="29" t="s">
+      <c r="A12" s="70"/>
+      <c r="B12" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="41" t="s">
+      <c r="F12" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="119">
         <v>10</v>
       </c>
-      <c r="I12" s="57">
+      <c r="I12" s="120">
         <v>30</v>
       </c>
       <c r="L12" s="11"/>
@@ -2024,29 +2117,29 @@
       <c r="AA12" s="11"/>
     </row>
     <row r="13" spans="1:27" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="88"/>
-      <c r="B13" s="30" t="s">
+      <c r="A13" s="77"/>
+      <c r="B13" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="121" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="122" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="123" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="G13" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="123">
         <v>10</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="124">
         <v>30</v>
       </c>
       <c r="L13" s="12"/>
@@ -2067,286 +2160,286 @@
       <c r="AA13" s="12"/>
     </row>
     <row r="14" spans="1:27" ht="147" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="111" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="112" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="112" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="125" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="97" t="s">
+      <c r="F14" s="126" t="s">
         <v>119</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="127" t="s">
         <v>120</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="114">
         <v>80</v>
       </c>
-      <c r="I14" s="56">
+      <c r="I14" s="116">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="161.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="87"/>
-      <c r="B15" s="92" t="s">
+      <c r="A15" s="70"/>
+      <c r="B15" s="128" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="117" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="119" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="99" t="s">
+      <c r="F15" s="130" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="100" t="s">
+      <c r="G15" s="127" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="119">
         <v>70</v>
       </c>
-      <c r="I15" s="57">
+      <c r="I15" s="120">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="88"/>
-      <c r="B16" s="93" t="s">
+      <c r="A16" s="77"/>
+      <c r="B16" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="D16" s="132" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="123" t="s">
         <v>124</v>
       </c>
-      <c r="F16" s="101" t="s">
+      <c r="F16" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="G16" s="102" t="s">
+      <c r="G16" s="127" t="s">
         <v>126</v>
       </c>
-      <c r="H16" s="42">
+      <c r="H16" s="123">
         <v>90</v>
       </c>
-      <c r="I16" s="58"/>
+      <c r="I16" s="124"/>
     </row>
     <row r="17" spans="1:9" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="86" t="s">
+      <c r="A17" s="134" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="112" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="112" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="94" t="s">
+      <c r="D17" s="125" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="114" t="s">
         <v>131</v>
       </c>
-      <c r="F17" s="97" t="s">
+      <c r="F17" s="126" t="s">
         <v>132</v>
       </c>
-      <c r="G17" s="98" t="s">
+      <c r="G17" s="127" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="114">
         <v>70</v>
       </c>
-      <c r="I17" s="56">
+      <c r="I17" s="116">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="134" t="s">
         <v>134</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="112" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="112" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="94" t="s">
+      <c r="D18" s="125" t="s">
         <v>137</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="97" t="s">
+      <c r="F18" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="127" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="114">
         <v>80</v>
       </c>
-      <c r="I18" s="56">
+      <c r="I18" s="116">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="134" t="s">
         <v>141</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="94" t="s">
+      <c r="D19" s="125" t="s">
         <v>144</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="114" t="s">
         <v>145</v>
       </c>
-      <c r="F19" s="97" t="s">
+      <c r="F19" s="126" t="s">
         <v>146</v>
       </c>
-      <c r="G19" s="98" t="s">
+      <c r="G19" s="127" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="114">
         <v>70</v>
       </c>
-      <c r="I19" s="56">
+      <c r="I19" s="116">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="134" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="112" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="112" t="s">
         <v>150</v>
       </c>
-      <c r="D20" s="94" t="s">
+      <c r="D20" s="125" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="114" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="97" t="s">
+      <c r="F20" s="126" t="s">
         <v>153</v>
       </c>
-      <c r="G20" s="98" t="s">
+      <c r="G20" s="127" t="s">
         <v>154</v>
       </c>
-      <c r="H20" s="40">
+      <c r="H20" s="114">
         <v>80</v>
       </c>
-      <c r="I20" s="56">
+      <c r="I20" s="116">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="134" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="94" t="s">
+      <c r="D21" s="125" t="s">
         <v>158</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="F21" s="97" t="s">
+      <c r="F21" s="126" t="s">
         <v>161</v>
       </c>
-      <c r="G21" s="98" t="s">
+      <c r="G21" s="127" t="s">
         <v>160</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H21" s="114">
         <v>90</v>
       </c>
-      <c r="I21" s="56">
+      <c r="I21" s="116">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="141.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="86" t="s">
+      <c r="A22" s="134" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="D22" s="94" t="s">
+      <c r="D22" s="125" t="s">
         <v>165</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="114" t="s">
         <v>166</v>
       </c>
-      <c r="F22" s="97" t="s">
+      <c r="F22" s="126" t="s">
         <v>167</v>
       </c>
-      <c r="G22" s="98" t="s">
+      <c r="G22" s="127" t="s">
         <v>168</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="114">
         <v>70</v>
       </c>
-      <c r="I22" s="56">
+      <c r="I22" s="116">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="163.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="86" t="s">
+      <c r="A23" s="134" t="s">
         <v>174</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="112" t="s">
         <v>175</v>
       </c>
-      <c r="D23" s="94" t="s">
+      <c r="D23" s="125" t="s">
         <v>170</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="114" t="s">
         <v>171</v>
       </c>
-      <c r="F23" s="97" t="s">
+      <c r="F23" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="G23" s="98" t="s">
+      <c r="G23" s="127" t="s">
         <v>173</v>
       </c>
-      <c r="H23" s="40">
+      <c r="H23" s="114">
         <v>80</v>
       </c>
-      <c r="I23" s="56">
+      <c r="I23" s="116">
         <v>50</v>
       </c>
     </row>
@@ -2403,14 +2496,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="39">
         <f t="shared" ref="B2:B13" si="0">D$1:D$13/C$1:C$13</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="41">
         <v>60</v>
       </c>
       <c r="D2" s="19">
@@ -2421,200 +2514,200 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="37">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="42">
         <v>40</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="53">
         <v>60</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="55" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="40">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="43">
         <v>50</v>
       </c>
-      <c r="D4" s="60">
+      <c r="D4" s="54">
         <v>40</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="54" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="38">
         <f t="shared" si="0"/>
         <v>0.8571428571428571</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="44">
         <v>70</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="20">
         <v>60</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="45">
         <v>80</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="21">
         <v>80</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="21" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="30">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="46">
         <v>90</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="27">
         <v>60</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="27" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="31">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C8" s="53">
+      <c r="C8" s="47">
         <v>60</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="28">
         <v>40</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="28" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="32">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="48">
         <v>50</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="22">
         <v>90</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="22" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="33">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="C10" s="55">
+      <c r="C10" s="49">
         <v>40</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="23">
         <v>60</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="23" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="34">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C11" s="56">
+      <c r="C11" s="50">
         <v>30</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="24">
         <v>60</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="51">
         <v>40</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="25">
         <v>40</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="36">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C13" s="58">
+      <c r="C13" s="52">
         <v>30</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="26">
         <v>20</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="26" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Contrat in every Axe + Dynamic
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E8BBA-F88D-4FB2-BD90-17086A234092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F281AA-0EB5-4996-8190-217A5D21E6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="184">
   <si>
     <t>Theme</t>
   </si>
@@ -384,9 +384,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t xml:space="preserve">  Complexity</t>
-  </si>
-  <si>
     <t xml:space="preserve">Priorité </t>
   </si>
   <si>
@@ -477,9 +474,6 @@
     <t>R-I-1</t>
   </si>
   <si>
-    <t>En tant qu'Agent Du Topnet, Établir la génération et la présentation des rapports suite au calcul des critères d'engagement client.</t>
-  </si>
-  <si>
     <t>Cette section concerne la génération et la présentation des rapports suite au calcul des critères d'engagement client. Les rapports doivent fournir des informations claires et détaillées sur les résultats de l'évaluation.</t>
   </si>
   <si>
@@ -501,9 +495,6 @@
     <t>B-I-1</t>
   </si>
   <si>
-    <t>En tant qu'Agent Du Topnet, Assurer la sauvegarde régulière et la gestion de l'historique des données du système.</t>
-  </si>
-  <si>
     <t>Cette section concerne la sauvegarde régulière et la gestion de l'historique des données du système. Les sauvegardes doivent être effectuées de manière sécurisée et périodique.</t>
   </si>
   <si>
@@ -525,9 +516,6 @@
     <t>S-I-1</t>
   </si>
   <si>
-    <t>En tant qu'Agent Du Topnet, Permettre la visualisation et la consultation des statistiques relatives à l'évolution des indicateurs clés de performance (KPI) du système.</t>
-  </si>
-  <si>
     <t>Cette section concerne la visualisation et la consultation des statistiques relatives à l'évolution des indicateurs clés de performance (KPI) du système.</t>
   </si>
   <si>
@@ -549,9 +537,6 @@
     <t>GS-I-1</t>
   </si>
   <si>
-    <t>En tant qu'Agent Du Topnet, Mettre en place la création de simulations basées sur différents scénarios pour évaluer l'impact des changements potentiels sur les performances du système.</t>
-  </si>
-  <si>
     <t>Cette section concerne la création de simulations basées sur différents scénarios pour évaluer l'impact des changements potentiels sur les performances du système.</t>
   </si>
   <si>
@@ -572,9 +557,6 @@
     <t>C-I-1</t>
   </si>
   <si>
-    <t>En tant qu'Agent Du Topnet,  Configurer les paramètres utilisés pour établir les scores d'engagement client et de comportement client.</t>
-  </si>
-  <si>
     <t>Cette section concerne la configuration des paramètres utilisés pour établir les scores d'engagement client et de comportement client.</t>
   </si>
   <si>
@@ -596,9 +578,6 @@
     <t>SDD-I-1</t>
   </si>
   <si>
-    <t>En tant qu'Agent Du Topnet,  Assurer la gestion et le stockage sécurisé des données clients et des résultats d'évaluation dans le système.</t>
-  </si>
-  <si>
     <t>Cette section concerne la gestion et le stockage sécurisé des données clients et des résultats d'évaluation dans le système.</t>
   </si>
   <si>
@@ -614,9 +593,6 @@
     <t xml:space="preserve">  Categorie Client</t>
   </si>
   <si>
-    <t>En tant qu'Agent Du Topnet, Mettre en place le classement et la catégorisation des clients en fonction de leur valeur commerciale, permettant un filtrage et un tri efficaces.</t>
-  </si>
-  <si>
     <t>Cette section concerne le classement et la catégorisation des clients en fonction de leur valeur commerciale, permettant un filtrage et un tri efficaces.</t>
   </si>
   <si>
@@ -633,6 +609,54 @@
   </si>
   <si>
     <t>CCL-I-1</t>
+  </si>
+  <si>
+    <t>En tant qu'Agent Du Topnet, je veux pouvoir Assurer la sauvegarde régulière et la gestion de l'historique des données du système.</t>
+  </si>
+  <si>
+    <t>En tant qu'Agent Du Topnet,je veux pouvoir Permettre la visualisation et la consultation des statistiques relatives à l'évolution des indicateurs clés de performance (KPI) du système.</t>
+  </si>
+  <si>
+    <t>En tant qu'Agent Du Topnet,je veux pouvoir Établir la génération et la présentation des rapports suite au calcul des critères d'engagement client.</t>
+  </si>
+  <si>
+    <t>En tant qu'Agent Du Topnet, je veux pouvoir Mettre en place la création de simulations basées sur différents scénarios pour évaluer l'impact des changements potentiels sur les performances du système.</t>
+  </si>
+  <si>
+    <t>En tant qu'Agent Du Topnet, je veux pouvoir  Configurer les paramètres utilisés pour établir les scores d'engagement client et de comportement client.</t>
+  </si>
+  <si>
+    <t>En tant qu'Agent Du Topnet,  je veux pouvoir Assurer la gestion et le stockage sécurisé des données clients et des résultats d'évaluation dans le système.</t>
+  </si>
+  <si>
+    <t>En tant qu'Agent Du Topnet, je veux pouvoir Mettre en place le classement et la catégorisation des clients en fonction de leur valeur commerciale, permettant un filtrage et un tri efficaces.</t>
+  </si>
+  <si>
+    <t>Complexite</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 8 </t>
   </si>
 </sst>
 </file>
@@ -653,11 +677,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color rgb="FFFFFFFF"/>
@@ -671,13 +690,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -707,13 +719,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -747,6 +752,26 @@
       <b/>
       <sz val="22"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -951,7 +976,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1107,256 +1132,323 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1582,10 +1674,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="58" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="72" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1597,8 +1689,7 @@
     <col min="5" max="5" width="149.85546875" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
     <col min="7" max="7" width="126.42578125" customWidth="1"/>
-    <col min="8" max="8" width="75.28515625" customWidth="1"/>
-    <col min="9" max="9" width="44.28515625" customWidth="1"/>
+    <col min="8" max="9" width="75.28515625" customWidth="1"/>
     <col min="10" max="10" width="47.85546875" customWidth="1"/>
     <col min="11" max="11" width="46.7109375" customWidth="1"/>
     <col min="12" max="27" width="14.42578125" hidden="1" customWidth="1"/>
@@ -1629,10 +1720,10 @@
         <v>79</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1652,32 +1743,38 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="61">
+      <c r="H2" s="123">
         <v>50</v>
       </c>
-      <c r="I2" s="63">
-        <v>60</v>
+      <c r="I2" s="131">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1697,30 +1794,36 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65" t="s">
+      <c r="A3" s="116"/>
+      <c r="B3" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="124">
         <v>40</v>
       </c>
-      <c r="I3" s="69">
-        <v>40</v>
+      <c r="I3" s="130">
+        <v>8</v>
+      </c>
+      <c r="J3" s="132">
+        <v>8</v>
+      </c>
+      <c r="K3" s="133" t="s">
+        <v>177</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1740,31 +1843,35 @@
       <c r="AA3" s="3"/>
     </row>
     <row r="4" spans="1:27" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71" t="s">
+      <c r="A4" s="117"/>
+      <c r="B4" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="73" t="s">
+      <c r="E4" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="74">
+      <c r="H4" s="125">
         <v>10</v>
       </c>
-      <c r="I4" s="76">
-        <v>50</v>
-      </c>
+      <c r="I4" s="129">
+        <v>2</v>
+      </c>
+      <c r="J4" s="132">
+        <v>2</v>
+      </c>
+      <c r="K4" s="133"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1783,31 +1890,35 @@
       <c r="AA4" s="4"/>
     </row>
     <row r="5" spans="1:27" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="77"/>
-      <c r="B5" s="78" t="s">
+      <c r="A5" s="118"/>
+      <c r="B5" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="80" t="s">
+      <c r="F5" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="80">
+      <c r="H5" s="126">
         <v>60</v>
       </c>
-      <c r="I5" s="82">
-        <v>70</v>
-      </c>
+      <c r="I5" s="128">
+        <v>27</v>
+      </c>
+      <c r="J5" s="132">
+        <v>8</v>
+      </c>
+      <c r="K5" s="133"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -1826,32 +1937,38 @@
       <c r="AA5" s="5"/>
     </row>
     <row r="6" spans="1:27" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="85" t="s">
+      <c r="D6" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="87" t="s">
+      <c r="G6" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="86">
+      <c r="H6" s="77">
         <v>70</v>
       </c>
-      <c r="I6" s="88">
-        <v>60</v>
+      <c r="I6" s="127">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" s="134" t="s">
+        <v>178</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -1871,58 +1988,66 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="7" spans="1:27" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="70"/>
-      <c r="B7" s="89" t="s">
+      <c r="A7" s="117"/>
+      <c r="B7" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="91" t="s">
+      <c r="D7" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="92">
+      <c r="H7" s="82">
         <v>30</v>
       </c>
-      <c r="I7" s="93">
-        <v>70</v>
-      </c>
+      <c r="I7" s="82">
+        <v>41</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7" s="134"/>
     </row>
     <row r="8" spans="1:27" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="77"/>
-      <c r="B8" s="94" t="s">
+      <c r="A8" s="118"/>
+      <c r="B8" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="97" t="s">
+      <c r="F8" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="98" t="s">
+      <c r="G8" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H8" s="86">
         <v>80</v>
       </c>
-      <c r="I8" s="99">
+      <c r="I8" s="86">
         <v>60</v>
       </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8" s="134"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -1941,33 +2066,37 @@
       <c r="AA8" s="7"/>
     </row>
     <row r="9" spans="1:27" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="102" t="s">
+      <c r="D9" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="103" t="s">
+      <c r="E9" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="103" t="s">
+      <c r="F9" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="104" t="s">
+      <c r="G9" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="103">
+      <c r="H9" s="90">
         <v>40</v>
       </c>
-      <c r="I9" s="105">
-        <v>50</v>
-      </c>
+      <c r="I9" s="90">
+        <v>76</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9" s="134"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -1986,30 +2115,36 @@
       <c r="AA9" s="8"/>
     </row>
     <row r="10" spans="1:27" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="77"/>
-      <c r="B10" s="106" t="s">
+      <c r="A10" s="118"/>
+      <c r="B10" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="107" t="s">
+      <c r="D10" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="108" t="s">
+      <c r="E10" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="108" t="s">
+      <c r="F10" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="109" t="s">
+      <c r="G10" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="108">
+      <c r="H10" s="94">
         <v>10</v>
       </c>
-      <c r="I10" s="110">
-        <v>40</v>
+      <c r="I10" s="94">
+        <v>54</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10" s="134" t="s">
+        <v>179</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
@@ -2029,33 +2164,37 @@
       <c r="AA10" s="9"/>
     </row>
     <row r="11" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="113" t="s">
+      <c r="D11" s="97" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="114" t="s">
+      <c r="E11" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="114" t="s">
+      <c r="F11" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="115" t="s">
+      <c r="G11" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="114">
+      <c r="H11" s="98">
         <v>20</v>
       </c>
-      <c r="I11" s="116">
-        <v>30</v>
-      </c>
+      <c r="I11" s="98">
+        <v>81</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11" s="134"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
@@ -2074,31 +2213,35 @@
       <c r="AA11" s="10"/>
     </row>
     <row r="12" spans="1:27" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="70"/>
-      <c r="B12" s="117" t="s">
+      <c r="A12" s="117"/>
+      <c r="B12" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="117" t="s">
+      <c r="C12" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="118" t="s">
+      <c r="D12" s="101" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="119" t="s">
+      <c r="E12" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="119" t="s">
+      <c r="F12" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="115" t="s">
+      <c r="G12" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="119">
+      <c r="H12" s="102">
         <v>10</v>
       </c>
-      <c r="I12" s="120">
-        <v>30</v>
-      </c>
+      <c r="I12" s="102">
+        <v>76</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12" s="134"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -2117,30 +2260,36 @@
       <c r="AA12" s="11"/>
     </row>
     <row r="13" spans="1:27" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="77"/>
-      <c r="B13" s="121" t="s">
+      <c r="A13" s="118"/>
+      <c r="B13" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="121" t="s">
+      <c r="C13" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="123" t="s">
+      <c r="E13" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="123" t="s">
+      <c r="F13" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="115" t="s">
+      <c r="G13" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="123">
+      <c r="H13" s="105">
         <v>10</v>
       </c>
-      <c r="I13" s="124">
-        <v>30</v>
+      <c r="I13" s="105">
+        <v>42</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13" s="134" t="s">
+        <v>180</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -2160,302 +2309,352 @@
       <c r="AA13" s="12"/>
     </row>
     <row r="14" spans="1:27" ht="147" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="121" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="112" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="112" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="125" t="s">
-        <v>115</v>
-      </c>
-      <c r="E14" s="114" t="s">
+      <c r="C14" s="96" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="106" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="107" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="126" t="s">
+      <c r="G14" s="108" t="s">
         <v>119</v>
       </c>
-      <c r="G14" s="127" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="114">
+      <c r="H14" s="98">
         <v>80</v>
       </c>
-      <c r="I14" s="116">
-        <v>60</v>
-      </c>
+      <c r="I14" s="98">
+        <v>87</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14" s="134"/>
     </row>
     <row r="15" spans="1:27" ht="161.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="70"/>
-      <c r="B15" s="128" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="117" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="129" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="119" t="s">
+      <c r="A15" s="117"/>
+      <c r="B15" s="109" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="100" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="110" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="102" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="111" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="130" t="s">
+      <c r="G15" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="127" t="s">
-        <v>123</v>
-      </c>
-      <c r="H15" s="119">
+      <c r="H15" s="102">
         <v>70</v>
       </c>
-      <c r="I15" s="120">
-        <v>50</v>
-      </c>
+      <c r="I15" s="102">
+        <v>65</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15" s="134"/>
     </row>
     <row r="16" spans="1:27" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="77"/>
-      <c r="B16" s="131" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="121" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="132" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="123" t="s">
+      <c r="A16" s="118"/>
+      <c r="B16" s="112" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="103" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="113" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="105" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="114" t="s">
         <v>124</v>
       </c>
-      <c r="F16" s="133" t="s">
+      <c r="G16" s="108" t="s">
         <v>125</v>
       </c>
-      <c r="G16" s="127" t="s">
+      <c r="H16" s="105">
+        <v>90</v>
+      </c>
+      <c r="I16" s="105">
+        <v>37</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+      <c r="K16" s="134" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="H16" s="123">
+      <c r="B17" s="96" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="96" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="98" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="107" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="108" t="s">
+        <v>131</v>
+      </c>
+      <c r="H17" s="98">
+        <v>70</v>
+      </c>
+      <c r="I17" s="98">
+        <v>58</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17" s="134"/>
+    </row>
+    <row r="18" spans="1:11" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="122" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="96" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="96" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="106" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="98" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="107" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="H18" s="98">
+        <v>80</v>
+      </c>
+      <c r="I18" s="98">
+        <v>27</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18" s="134"/>
+    </row>
+    <row r="19" spans="1:11" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="122" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="96" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="96" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="106" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="98" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="107" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="108" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="98">
+        <v>70</v>
+      </c>
+      <c r="I19" s="98">
+        <v>87</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19" s="134" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="122" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="96" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="96" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="106" t="s">
+        <v>171</v>
+      </c>
+      <c r="E20" s="98" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="G20" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="98">
+        <v>80</v>
+      </c>
+      <c r="I20" s="98">
+        <v>55</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20" s="134"/>
+    </row>
+    <row r="21" spans="1:11" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="122" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="96" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="106" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="98" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" s="108" t="s">
+        <v>154</v>
+      </c>
+      <c r="H21" s="98">
         <v>90</v>
       </c>
-      <c r="I16" s="124"/>
+      <c r="I21" s="98">
+        <v>42</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21" s="134"/>
     </row>
-    <row r="17" spans="1:9" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="134" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="112" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="112" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="125" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="114" t="s">
-        <v>131</v>
-      </c>
-      <c r="F17" s="126" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="127" t="s">
-        <v>133</v>
-      </c>
-      <c r="H17" s="114">
+    <row r="22" spans="1:11" ht="141.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="96" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="96" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="106" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="98" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" s="107" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="108" t="s">
+        <v>161</v>
+      </c>
+      <c r="H22" s="98">
         <v>70</v>
       </c>
-      <c r="I17" s="116">
-        <v>60</v>
+      <c r="I22" s="98">
+        <v>14</v>
+      </c>
+      <c r="J22">
+        <v>8</v>
+      </c>
+      <c r="K22" s="134" t="s">
+        <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="134" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>135</v>
-      </c>
-      <c r="C18" s="112" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" s="125" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" s="114" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" s="126" t="s">
-        <v>139</v>
-      </c>
-      <c r="G18" s="127" t="s">
-        <v>140</v>
-      </c>
-      <c r="H18" s="114">
+    <row r="23" spans="1:11" ht="163.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="122" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" s="96" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="96" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="106" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="98" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" s="107" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="108" t="s">
+        <v>165</v>
+      </c>
+      <c r="H23" s="98">
         <v>80</v>
       </c>
-      <c r="I18" s="116">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="134" t="s">
-        <v>141</v>
-      </c>
-      <c r="B19" s="112" t="s">
-        <v>142</v>
-      </c>
-      <c r="C19" s="112" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="125" t="s">
-        <v>144</v>
-      </c>
-      <c r="E19" s="114" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" s="126" t="s">
-        <v>146</v>
-      </c>
-      <c r="G19" s="127" t="s">
-        <v>147</v>
-      </c>
-      <c r="H19" s="114">
-        <v>70</v>
-      </c>
-      <c r="I19" s="116">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="134" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="112" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="112" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="125" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="114" t="s">
-        <v>152</v>
-      </c>
-      <c r="F20" s="126" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" s="127" t="s">
-        <v>154</v>
-      </c>
-      <c r="H20" s="114">
-        <v>80</v>
-      </c>
-      <c r="I20" s="116">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="134" t="s">
-        <v>155</v>
-      </c>
-      <c r="B21" s="112" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" s="112" t="s">
-        <v>157</v>
-      </c>
-      <c r="D21" s="125" t="s">
-        <v>158</v>
-      </c>
-      <c r="E21" s="114" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" s="126" t="s">
-        <v>161</v>
-      </c>
-      <c r="G21" s="127" t="s">
-        <v>160</v>
-      </c>
-      <c r="H21" s="114">
-        <v>90</v>
-      </c>
-      <c r="I21" s="116">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="141.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="134" t="s">
-        <v>162</v>
-      </c>
-      <c r="B22" s="112" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="112" t="s">
-        <v>164</v>
-      </c>
-      <c r="D22" s="125" t="s">
-        <v>165</v>
-      </c>
-      <c r="E22" s="114" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="126" t="s">
-        <v>167</v>
-      </c>
-      <c r="G22" s="127" t="s">
-        <v>168</v>
-      </c>
-      <c r="H22" s="114">
-        <v>70</v>
-      </c>
-      <c r="I22" s="116">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="163.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="134" t="s">
-        <v>174</v>
-      </c>
-      <c r="B23" s="112" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" s="112" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" s="125" t="s">
-        <v>170</v>
-      </c>
-      <c r="E23" s="114" t="s">
-        <v>171</v>
-      </c>
-      <c r="F23" s="126" t="s">
-        <v>172</v>
-      </c>
-      <c r="G23" s="127" t="s">
-        <v>173</v>
-      </c>
-      <c r="H23" s="114">
-        <v>80</v>
-      </c>
-      <c r="I23" s="116">
-        <v>50</v>
-      </c>
+      <c r="I23" s="98">
+        <v>41</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23" s="134"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="12">
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="K6:K9"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="K16:K18"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I23" xr:uid="{86B5F61D-41F8-4621-A960-58147D9E9B9D}">
-      <formula1>"10,20,30,40,50,60,70,80,90,100"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix backlog / sprint backlog
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F281AA-0EB5-4996-8190-217A5D21E6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720B5C52-F8D5-4C06-B2E6-120081B3B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="171">
   <si>
     <t>Theme</t>
   </si>
@@ -393,21 +393,11 @@
     <t>Authentification de l'Agent</t>
   </si>
   <si>
-    <t xml:space="preserve">Authentification du Client
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gestion des comptes d'utilisateur
 </t>
   </si>
   <si>
     <t>A-I-1</t>
-  </si>
-  <si>
-    <t>A-I-2</t>
-  </si>
-  <si>
-    <t>A-I-3</t>
   </si>
   <si>
     <t>En tant qu'Agent Du Topnet, je veux pouvoir m'authentifier avec mon identifiant et mon mot de passe pour accéder au système.
@@ -415,11 +405,6 @@
 En tant qu'Agent Du Topnet, je veux avoir la possibilité de récupérer mon mot de passe en cas d'oubli via une réinitialisation sécurisée.</t>
   </si>
   <si>
-    <t>En tant que client de Topnet, je veux pouvoir m'authentifier avec mon identifiant et mon mot de passe pour accéder à mon compte en ligne.
-En tant que client de Topnet, je veux pouvoir me déconnecter facilement de mon compte pour assurer la sécurité de mes informations personnelles.
-En tant que client de Topnet, je veux être informé en cas d'échec de l'authentification pour éviter les tentatives d'accès non autorisées.</t>
-  </si>
-  <si>
     <t>En tant qu'Administrateur du système, je veux pouvoir gérer les comptes des agents, y compris la création, la modification et la suppression des comptes.
 En tant qu'Administrateur du système, je veux pouvoir attribuer des rôles et des autorisations spécifiques à chaque compte d'agent pour contrôler l'accès aux fonctionnalités du système.</t>
   </si>
@@ -434,18 +419,6 @@
     <t>L'agent peut se connecter avec succès en utilisant les bonnes informations d'identification.
 Un message d'erreur approprié est affiché en cas d'échec de l'authentification.
 L'agent peut demander une réinitialisation de mot de passe en cas d'oubli.</t>
-  </si>
-  <si>
-    <t>Cette section concerne l'authentification des clients du service en ligne de Topnet. Les clients doivent pouvoir accéder à leur compte en utilisant leurs identifiants et mots de passe.</t>
-  </si>
-  <si>
-    <t>Identifiant du Client
-Mot de passe du Client</t>
-  </si>
-  <si>
-    <t>Le client peut se connecter avec succès en utilisant les bonnes informations d'identification.
-Le client peut se déconnecter facilement de son compte.
-Un message d'erreur est affiché en cas d'échec de l'authentification.</t>
   </si>
   <si>
     <t>Cette section concerne la gestion des comptes des agents par l'administrateur du système.</t>
@@ -635,35 +608,17 @@
     <t>Complexite</t>
   </si>
   <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 8 </t>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>A-I-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +727,21 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -976,7 +946,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1192,14 +1162,90 @@
       </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1399,15 +1445,6 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1416,21 +1453,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1444,11 +1466,66 @@
     <xf numFmtId="0" fontId="4" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1674,15 +1751,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="72" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="72" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" customWidth="1"/>
+    <col min="1" max="1" width="80.7109375" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" customWidth="1"/>
     <col min="4" max="4" width="240" customWidth="1"/>
@@ -1690,14 +1767,13 @@
     <col min="6" max="6" width="59" customWidth="1"/>
     <col min="7" max="7" width="126.42578125" customWidth="1"/>
     <col min="8" max="9" width="75.28515625" customWidth="1"/>
-    <col min="10" max="10" width="47.85546875" customWidth="1"/>
-    <col min="11" max="11" width="46.7109375" customWidth="1"/>
-    <col min="12" max="27" width="14.42578125" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="145.140625" customWidth="1"/>
-    <col min="29" max="29" width="64.28515625" customWidth="1"/>
+    <col min="10" max="10" width="46.7109375" customWidth="1"/>
+    <col min="11" max="26" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="145.140625" customWidth="1"/>
+    <col min="28" max="28" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
@@ -1723,8 +1799,12 @@
         <v>106</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>175</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="J1" s="122" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1740,10 +1820,9 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="115" t="s">
+    <row r="2" spans="1:26" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="139" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="57" t="s">
@@ -1764,18 +1843,14 @@
       <c r="G2" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="123">
+      <c r="H2" s="113">
         <v>50</v>
       </c>
-      <c r="I2" s="131">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>176</v>
-      </c>
+      <c r="I2" s="121">
+        <v>4</v>
+      </c>
+      <c r="J2" s="136"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1791,10 +1866,9 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
     </row>
-    <row r="3" spans="1:27" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="116"/>
+    <row r="3" spans="1:26" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="140"/>
       <c r="B3" s="62" t="s">
         <v>6</v>
       </c>
@@ -1813,18 +1887,16 @@
       <c r="G3" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="124">
+      <c r="H3" s="114">
         <v>40</v>
       </c>
-      <c r="I3" s="130">
+      <c r="I3" s="120">
         <v>8</v>
       </c>
-      <c r="J3" s="132">
-        <v>8</v>
-      </c>
-      <c r="K3" s="133" t="s">
-        <v>177</v>
-      </c>
+      <c r="J3" s="135">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -1840,10 +1912,9 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="117"/>
+    <row r="4" spans="1:26" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="141"/>
       <c r="B4" s="66" t="s">
         <v>7</v>
       </c>
@@ -1862,16 +1933,14 @@
       <c r="G4" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="125">
+      <c r="H4" s="115">
         <v>10</v>
       </c>
-      <c r="I4" s="129">
+      <c r="I4" s="119">
         <v>2</v>
       </c>
-      <c r="J4" s="132">
-        <v>2</v>
-      </c>
-      <c r="K4" s="133"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1887,10 +1956,9 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="1:27" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="118"/>
+    <row r="5" spans="1:26" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="142"/>
       <c r="B5" s="71" t="s">
         <v>8</v>
       </c>
@@ -1909,16 +1977,14 @@
       <c r="G5" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="126">
+      <c r="H5" s="116">
         <v>60</v>
       </c>
-      <c r="I5" s="128">
-        <v>27</v>
-      </c>
-      <c r="J5" s="132">
-        <v>8</v>
-      </c>
-      <c r="K5" s="133"/>
+      <c r="I5" s="118">
+        <v>2</v>
+      </c>
+      <c r="J5" s="128"/>
+      <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -1934,10 +2000,9 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
     </row>
-    <row r="6" spans="1:27" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="119" t="s">
+    <row r="6" spans="1:26" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="143" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="75" t="s">
@@ -1961,15 +2026,11 @@
       <c r="H6" s="77">
         <v>70</v>
       </c>
-      <c r="I6" s="127">
-        <v>30</v>
-      </c>
-      <c r="J6">
+      <c r="I6" s="117">
         <v>2</v>
       </c>
-      <c r="K6" s="134" t="s">
-        <v>178</v>
-      </c>
+      <c r="J6" s="123"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -1985,10 +2046,9 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
     </row>
-    <row r="7" spans="1:27" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="117"/>
+    <row r="7" spans="1:26" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="141"/>
       <c r="B7" s="79" t="s">
         <v>11</v>
       </c>
@@ -2011,15 +2071,14 @@
         <v>30</v>
       </c>
       <c r="I7" s="82">
-        <v>41</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7" s="134"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="133">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="1:27" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="118"/>
+    <row r="8" spans="1:26" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="142"/>
       <c r="B8" s="83" t="s">
         <v>12</v>
       </c>
@@ -2042,12 +2101,10 @@
         <v>80</v>
       </c>
       <c r="I8" s="86">
-        <v>60</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
-      <c r="K8" s="134"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="132"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -2063,10 +2120,9 @@
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:27" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="120" t="s">
+    <row r="9" spans="1:26" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="144" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="88" t="s">
@@ -2091,12 +2147,12 @@
         <v>40</v>
       </c>
       <c r="I9" s="90">
-        <v>76</v>
-      </c>
-      <c r="J9">
         <v>8</v>
       </c>
-      <c r="K9" s="134"/>
+      <c r="J9" s="124">
+        <v>3</v>
+      </c>
+      <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -2112,10 +2168,9 @@
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
     </row>
-    <row r="10" spans="1:27" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="118"/>
+    <row r="10" spans="1:26" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="142"/>
       <c r="B10" s="92" t="s">
         <v>40</v>
       </c>
@@ -2138,14 +2193,10 @@
         <v>10</v>
       </c>
       <c r="I10" s="94">
-        <v>54</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10" s="134" t="s">
-        <v>179</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J10" s="131"/>
+      <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -2161,10 +2212,9 @@
       <c r="X10" s="9"/>
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
     </row>
-    <row r="11" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="121" t="s">
+    <row r="11" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="145" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="96" t="s">
@@ -2189,12 +2239,10 @@
         <v>20</v>
       </c>
       <c r="I11" s="98">
-        <v>81</v>
-      </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11" s="134"/>
+        <v>4</v>
+      </c>
+      <c r="J11" s="125"/>
+      <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
@@ -2210,10 +2258,9 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AA11" s="10"/>
     </row>
-    <row r="12" spans="1:27" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="117"/>
+    <row r="12" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="141"/>
       <c r="B12" s="100" t="s">
         <v>16</v>
       </c>
@@ -2236,12 +2283,12 @@
         <v>10</v>
       </c>
       <c r="I12" s="102">
-        <v>76</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-      <c r="K12" s="134"/>
+        <v>10</v>
+      </c>
+      <c r="J12" s="129">
+        <v>4</v>
+      </c>
+      <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -2257,10 +2304,9 @@
       <c r="X12" s="11"/>
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
     </row>
-    <row r="13" spans="1:27" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="118"/>
+    <row r="13" spans="1:26" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="142"/>
       <c r="B13" s="103" t="s">
         <v>17</v>
       </c>
@@ -2283,14 +2329,10 @@
         <v>10</v>
       </c>
       <c r="I13" s="105">
-        <v>42</v>
-      </c>
-      <c r="J13">
-        <v>8</v>
-      </c>
-      <c r="K13" s="134" t="s">
-        <v>180</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J13" s="130"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
@@ -2306,354 +2348,290 @@
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
     </row>
-    <row r="14" spans="1:27" ht="147" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="121" t="s">
+    <row r="14" spans="1:26" ht="147" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="145" t="s">
         <v>107</v>
       </c>
       <c r="B14" s="96" t="s">
         <v>108</v>
       </c>
       <c r="C14" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="106" t="s">
+      <c r="E14" s="98" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="107" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="98" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="107" t="s">
-        <v>118</v>
-      </c>
       <c r="G14" s="108" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H14" s="98">
         <v>80</v>
       </c>
       <c r="I14" s="98">
-        <v>87</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14" s="134"/>
+        <v>8</v>
+      </c>
+      <c r="J14" s="126">
+        <v>5</v>
+      </c>
     </row>
-    <row r="15" spans="1:27" ht="161.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="117"/>
+    <row r="15" spans="1:26" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="142"/>
       <c r="B15" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="100" t="s">
+      <c r="C15" s="103" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="110" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="102" t="s">
+      <c r="E15" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="111" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="108" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="105">
+        <v>90</v>
+      </c>
+      <c r="I15" s="138">
+        <v>12</v>
+      </c>
+      <c r="J15" s="127"/>
+    </row>
+    <row r="16" spans="1:26" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="96" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="111" t="s">
+      <c r="C16" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="G15" s="108" t="s">
+      <c r="D16" s="106" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="H15" s="102">
+      <c r="F16" s="107" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="108" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="98">
         <v>70</v>
       </c>
-      <c r="I15" s="102">
-        <v>65</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
-      </c>
-      <c r="K15" s="134"/>
+      <c r="I16" s="137">
+        <v>10</v>
+      </c>
+      <c r="J16" s="126">
+        <v>6</v>
+      </c>
     </row>
-    <row r="16" spans="1:27" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="118"/>
-      <c r="B16" s="112" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" s="103" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="113" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="F16" s="114" t="s">
-        <v>124</v>
-      </c>
-      <c r="G16" s="108" t="s">
+    <row r="17" spans="1:10" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="112" t="s">
         <v>125</v>
       </c>
-      <c r="H16" s="105">
-        <v>90</v>
-      </c>
-      <c r="I16" s="105">
-        <v>37</v>
-      </c>
-      <c r="J16">
+      <c r="B17" s="96" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="96" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="98" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" s="98">
+        <v>80</v>
+      </c>
+      <c r="I17" s="137">
         <v>8</v>
       </c>
-      <c r="K16" s="134" t="s">
-        <v>181</v>
-      </c>
+      <c r="J17" s="128"/>
     </row>
-    <row r="17" spans="1:11" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="122" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="96" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="96" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" s="106" t="s">
-        <v>170</v>
-      </c>
-      <c r="E17" s="98" t="s">
-        <v>129</v>
-      </c>
-      <c r="F17" s="107" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" s="108" t="s">
+    <row r="18" spans="1:10" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="H17" s="98">
+      <c r="B18" s="96" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="96" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="106" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="98" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="107" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="H18" s="98">
         <v>70</v>
       </c>
-      <c r="I17" s="98">
-        <v>58</v>
-      </c>
-      <c r="J17">
-        <v>3</v>
-      </c>
-      <c r="K17" s="134"/>
+      <c r="I18" s="98">
+        <v>4</v>
+      </c>
+      <c r="J18" s="127">
+        <v>7</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="122" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" s="96" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="96" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="106" t="s">
-        <v>168</v>
-      </c>
-      <c r="E18" s="98" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="107" t="s">
-        <v>136</v>
-      </c>
-      <c r="G18" s="108" t="s">
+    <row r="19" spans="1:10" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="112" t="s">
         <v>137</v>
       </c>
-      <c r="H18" s="98">
+      <c r="B19" s="96" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="96" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="106" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="98" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="108" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="98">
         <v>80</v>
       </c>
-      <c r="I18" s="98">
-        <v>27</v>
-      </c>
-      <c r="J18">
-        <v>5</v>
-      </c>
-      <c r="K18" s="134"/>
+      <c r="I19" s="98">
+        <v>6</v>
+      </c>
+      <c r="J19" s="127"/>
     </row>
-    <row r="19" spans="1:11" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="122" t="s">
-        <v>138</v>
-      </c>
-      <c r="B19" s="96" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="96" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="106" t="s">
-        <v>169</v>
-      </c>
-      <c r="E19" s="98" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="107" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="108" t="s">
+    <row r="20" spans="1:10" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="H19" s="98">
-        <v>70</v>
-      </c>
-      <c r="I19" s="98">
-        <v>87</v>
-      </c>
-      <c r="J19">
-        <v>8</v>
-      </c>
-      <c r="K19" s="134" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="122" t="s">
+      <c r="B20" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="96" t="s">
+      <c r="C20" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="96" t="s">
+      <c r="D20" s="106" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="98" t="s">
         <v>146</v>
-      </c>
-      <c r="D20" s="106" t="s">
-        <v>171</v>
-      </c>
-      <c r="E20" s="98" t="s">
-        <v>147</v>
       </c>
       <c r="F20" s="107" t="s">
         <v>148</v>
       </c>
       <c r="G20" s="108" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" s="98">
+        <v>90</v>
+      </c>
+      <c r="I20" s="98">
+        <v>8</v>
+      </c>
+      <c r="J20" s="127"/>
+    </row>
+    <row r="21" spans="1:10" ht="141.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="112" t="s">
         <v>149</v>
       </c>
-      <c r="H20" s="98">
-        <v>80</v>
-      </c>
-      <c r="I20" s="98">
-        <v>55</v>
-      </c>
-      <c r="J20">
-        <v>3</v>
-      </c>
-      <c r="K20" s="134"/>
-    </row>
-    <row r="21" spans="1:11" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="122" t="s">
+      <c r="B21" s="96" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="C21" s="96" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="D21" s="106" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="D21" s="106" t="s">
-        <v>172</v>
-      </c>
-      <c r="E21" s="98" t="s">
+      <c r="F21" s="107" t="s">
         <v>153</v>
-      </c>
-      <c r="F21" s="107" t="s">
-        <v>155</v>
       </c>
       <c r="G21" s="108" t="s">
         <v>154</v>
       </c>
       <c r="H21" s="98">
-        <v>90</v>
-      </c>
-      <c r="I21" s="98">
-        <v>42</v>
-      </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-      <c r="K21" s="134"/>
+        <v>70</v>
+      </c>
+      <c r="I21" s="137">
+        <v>6</v>
+      </c>
+      <c r="J21" s="126">
+        <v>8</v>
+      </c>
     </row>
-    <row r="22" spans="1:11" ht="141.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="122" t="s">
+    <row r="22" spans="1:10" ht="163.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="112" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="96" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="106" t="s">
+        <v>167</v>
+      </c>
+      <c r="E22" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="F22" s="107" t="s">
         <v>157</v>
       </c>
-      <c r="C22" s="96" t="s">
+      <c r="G22" s="108" t="s">
         <v>158</v>
       </c>
-      <c r="D22" s="106" t="s">
-        <v>173</v>
-      </c>
-      <c r="E22" s="98" t="s">
-        <v>159</v>
-      </c>
-      <c r="F22" s="107" t="s">
-        <v>160</v>
-      </c>
-      <c r="G22" s="108" t="s">
-        <v>161</v>
-      </c>
       <c r="H22" s="98">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I22" s="98">
-        <v>14</v>
-      </c>
-      <c r="J22">
-        <v>8</v>
-      </c>
-      <c r="K22" s="134" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="163.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="122" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="96" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="96" t="s">
-        <v>167</v>
-      </c>
-      <c r="D23" s="106" t="s">
-        <v>174</v>
-      </c>
-      <c r="E23" s="98" t="s">
-        <v>163</v>
-      </c>
-      <c r="F23" s="107" t="s">
-        <v>164</v>
-      </c>
-      <c r="G23" s="108" t="s">
-        <v>165</v>
-      </c>
-      <c r="H23" s="98">
-        <v>80</v>
-      </c>
-      <c r="I23" s="98">
-        <v>41</v>
-      </c>
-      <c r="J23">
-        <v>5</v>
-      </c>
-      <c r="K23" s="134"/>
+        <v>4</v>
+      </c>
+      <c r="J22" s="130"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="K6:K9"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="K16:K18"/>
+  <mergeCells count="5">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>